<commit_message>
Fixes for PLP module with page layout
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PlpTestData.xlsx
+++ b/src/test/resources/TestData/PlpTestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJI-GOA-70\Downloads\template-selenium-main\template-selenium-main\Neostrata\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadee\git\Neostrata\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD47D517-3B58-4054-924B-F13A6206238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE82E614-4FBC-4171-B792-8C80F272772A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="996" yWindow="1332" windowWidth="20784" windowHeight="11256" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sort" sheetId="1" r:id="rId1"/>
     <sheet name="category" sheetId="2" r:id="rId2"/>
-    <sheet name="ingredients" sheetId="3" r:id="rId3"/>
+    <sheet name="pageLayout" sheetId="6" r:id="rId3"/>
+    <sheet name="ingredients" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
   <si>
     <t>TestCase</t>
   </si>
@@ -77,18 +78,12 @@
     <t>Option</t>
   </si>
   <si>
-    <t>ExpResult</t>
-  </si>
-  <si>
     <t>https://www.neostrata.com/collections/cleansers</t>
   </si>
   <si>
     <t>Verify the dropdown category 'Cleanser' dropdown</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Cleansers</t>
   </si>
   <si>
@@ -173,20 +168,185 @@
     <t>https://www.neostrata.com/collections/value-sets</t>
   </si>
   <si>
-    <t>Verify the ingredients Product listing page</t>
-  </si>
-  <si>
-    <t>MicroDiPeptide229</t>
-  </si>
-  <si>
-    <t>ingredients</t>
+    <t>Verify the MicroDiPeptide229 Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Vitamin C Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Glycolic Acid Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Hyaluronic Acid Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Gluconolactone Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Retinol Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the NeoGlucosamine Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the NeoCitriate Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Salicylic Acid Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Poly Hydroxy Acids (PHA) Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Alpha Hydroxy Acids (AHA) Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Vitamin E Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the SPF Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Peptides Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Niacinamide Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Antioxidants Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Green Tea Extract Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Aminofil Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Mandelic Acid Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Tranexamic Acid Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the AHA/PHA Blend (including Mandelic Acid) Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Alpine Plant Extract Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Antiaging Peptide Complex Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Botancial Blend Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Green Tea Extract, Chamomile &amp; Calendula Extracts Product listing page</t>
+  </si>
+  <si>
+    <t>Verify the Vitamin C &amp; E Product listing page</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67535106&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>expectedResult</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67698946&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67305730&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67731714&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F93946114&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67567874&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67666178&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67961090&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67862786&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67764482&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67797250&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67633410&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F68026626&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67895554&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67928322&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F75006210&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67993858&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67502338&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67600642&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FFilterSettingGroup%2F67830018&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F101090066690&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F101090164994&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F96918864130&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F101090230530&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F101378982146&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F99995320578&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F100023861506&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F101378916610&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/bestsellers?filter.p.m.custom.key_ingredients=gid%3A%2F%2Fshopify%2FMetaobject%2F99995287810&amp;sort_by=manual</t>
+  </si>
+  <si>
+    <t>breadcrumbcount</t>
+  </si>
+  <si>
+    <t>Check if breadcrumb is present</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,8 +378,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +413,12 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -246,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -285,6 +474,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,7 +762,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -606,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>14</v>
@@ -626,7 +819,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>14</v>
@@ -646,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>14</v>
@@ -675,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2959B7-E078-4CF8-8662-06C0DF4AF168}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -708,12 +901,12 @@
         <v>15</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2">
       <c r="A2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
@@ -725,15 +918,15 @@
         <v>6</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>5</v>
@@ -745,15 +938,15 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2">
       <c r="A4" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
@@ -765,15 +958,15 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2">
       <c r="A5" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>5</v>
@@ -785,15 +978,15 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2">
       <c r="A6" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>5</v>
@@ -805,15 +998,15 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2">
       <c r="A7" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>5</v>
@@ -825,15 +1018,15 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2">
       <c r="A8" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>5</v>
@@ -845,15 +1038,15 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2">
       <c r="A9" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>5</v>
@@ -865,15 +1058,15 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2">
       <c r="A10" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>5</v>
@@ -885,15 +1078,15 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2">
       <c r="A11" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>5</v>
@@ -905,14 +1098,11 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="F12" s="3"/>
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -941,18 +1131,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40927B92-654F-4363-9300-D083CEE741F3}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A45DC4-1E70-419B-AAB1-2563F966BCEA}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AE4786-B8CD-4624-9B6A-05C428C7C5C4}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="63.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="144.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -966,24 +1201,448 @@
         <v>7</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5F9E9A93-F1E9-480E-B5EE-68C3065914C2}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{7E4D5C69-EBB0-459E-B607-4202C13FE095}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{71922D0F-6377-4B1C-9298-4E50EEBE5EC8}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{949E7BD9-0A2B-43BB-ABED-DE01DE912C2F}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{D0034EF5-BF96-4C7E-8AD5-A3DEDE36CEE9}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{2A187C00-1083-4DA0-8BA8-B59E51B38C3E}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{94173357-2383-40DC-8D94-AB2328A4D1B7}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{4E9E718B-389D-4874-A9D6-A83E28E5F290}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{02966992-73C2-4F80-A281-692BA14F423D}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{215456CB-791C-49ED-9ABC-754D7EBFD5E6}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{631BE1DE-1B11-4DFB-9D09-197AF5DF441C}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{6B75791B-DA66-410F-8F11-2A3ABEFBC54F}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{1AC5AF6B-242F-4E84-8583-82F5C92F6E62}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{FC4EBC21-DD75-46C5-9685-942A75CB872A}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{75B938EA-B75B-4A27-BBF8-F7DDC95C01B5}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{935714BA-E841-4600-ACF9-4D8906B8CED1}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{902202CA-514E-421E-9B6E-5E34AB2C5981}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{DBE28D7D-CC64-4850-A86A-2F7DB0AD3858}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{4B93A8B4-62BD-4CAE-9D82-D696A9F1A8DB}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{F90CB230-C1DA-4A03-889C-7D068F87CF0C}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{6AC26EB5-E1B6-474A-BB3C-262665588DA0}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{6895D41D-2895-402D-A8E4-781F0D840546}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{B8778EBD-B0B8-44E2-8FEB-C205200310BA}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{B6E9645B-B7D3-4CB9-9801-B9622E4E07C0}"/>
+    <hyperlink ref="D26" r:id="rId25" xr:uid="{9A1225F4-79D7-401B-97CE-B4130D7B52F5}"/>
+    <hyperlink ref="D27" r:id="rId26" xr:uid="{7609ACAC-D06F-4796-8E4F-CC794EC5D7D6}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{673719D5-13B3-47C8-AE0F-A6E9FFA1549B}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{10C48C5A-BF49-4404-AC4E-1D0822D3C9C5}"/>
+    <hyperlink ref="D30" r:id="rId29" xr:uid="{650D7479-577D-4827-82B3-E1870C9E930C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>